<commit_message>
Completed AFOLU model. Ref includes new fake data complete.
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_en_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_en_demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4604496-A088-D94F-9902-2C5BCA739B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC2605A-202C-6041-B8E1-56033FCCE2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="460" windowWidth="23020" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2364,8 +2364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS587"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="107" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="A393" zoomScale="107" workbookViewId="0">
+      <selection activeCell="J415" sqref="J415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -52547,112 +52547,112 @@
         <v>1</v>
       </c>
       <c r="J412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="K412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="L412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="M412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="N412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="O412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="P412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="Q412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="R412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="S412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="T412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="U412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="V412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="W412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="X412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="Y412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="Z412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AA412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AB412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AC412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AD412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AE412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AF412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AG412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AH412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AI412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AJ412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AK412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AL412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AM412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AN412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AO412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AP412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AQ412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AR412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AS412">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
     </row>
     <row r="413" spans="1:45" x14ac:dyDescent="0.2">
@@ -52669,112 +52669,112 @@
         <v>1</v>
       </c>
       <c r="J413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="K413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="L413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="M413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="N413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="O413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="P413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="Q413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="R413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="S413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="T413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="U413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="V413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="W413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="X413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="Y413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="Z413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AA413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AB413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AC413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AD413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AE413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AF413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AG413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AH413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AI413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AJ413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AK413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AL413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AM413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AN413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AO413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AP413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AQ413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AR413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
       <c r="AS413">
-        <v>0.35299999999999998</v>
+        <v>0.30695652173913052</v>
       </c>
     </row>
     <row r="414" spans="1:45" x14ac:dyDescent="0.2">
@@ -52913,112 +52913,112 @@
         <v>1</v>
       </c>
       <c r="J415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="K415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="L415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="M415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="N415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="O415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="P415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="Q415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="R415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="S415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="T415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="U415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="V415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="W415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="X415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="Y415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="Z415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AA415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AB415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AC415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AD415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AE415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AF415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AG415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AH415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AI415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AJ415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AK415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AL415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AM415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AN415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AO415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AP415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AQ415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AR415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
       <c r="AS415">
-        <v>0.28899999999999998</v>
+        <v>0.25130434782608702</v>
       </c>
     </row>
     <row r="416" spans="1:45" x14ac:dyDescent="0.2">
@@ -53279,112 +53279,112 @@
         <v>1</v>
       </c>
       <c r="J418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="K418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="L418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="M418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="N418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="O418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="P418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="Q418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="R418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="S418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="T418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="U418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="V418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="W418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="X418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="Y418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="Z418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AA418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AB418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AC418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AD418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AE418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AF418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AG418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AH418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AI418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AJ418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AK418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AL418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AM418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AN418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AO418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AP418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AQ418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AR418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
       <c r="AS418">
-        <v>6.9000000000000006E-2</v>
+        <v>6.0000000000000019E-2</v>
       </c>
     </row>
     <row r="419" spans="1:45" x14ac:dyDescent="0.2">
@@ -53401,112 +53401,112 @@
         <v>1</v>
       </c>
       <c r="J419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="K419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="L419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="M419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="N419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="O419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="P419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="Q419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="R419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="S419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="T419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="U419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="V419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="W419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="X419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="Y419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="Z419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AA419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AB419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AC419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AD419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AE419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AF419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AG419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AH419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AI419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AJ419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AK419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AL419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AM419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AN419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AO419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AP419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AQ419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AR419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
       <c r="AS419">
-        <v>0</v>
+        <v>0.13043478260869568</v>
       </c>
     </row>
     <row r="420" spans="1:45" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
some changes to afolu
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_en_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_en_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8A57DE-01B0-8740-9E87-D52CAB725AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5727C72-C247-9941-91AF-5222A6164587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="460" windowWidth="23460" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3188,7 +3188,7 @@
   <dimension ref="A1:AS851"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B222" zoomScale="107" workbookViewId="0">
-      <selection activeCell="O264" sqref="O264"/>
+      <selection activeCell="B235" sqref="B235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>